<commit_message>
worked on inventory bugs solve
</commit_message>
<xml_diff>
--- a/dataTemplate/itemsExcelSample.xlsx
+++ b/dataTemplate/itemsExcelSample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Category</t>
   </si>
@@ -56,28 +56,19 @@
     <t>SGST</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>CIVIL MATERIAL</t>
   </si>
   <si>
-    <t>AAC BLOCK</t>
-  </si>
-  <si>
-    <t>AAC FLY ASH BLOCKS(600*200*150) 2</t>
-  </si>
-  <si>
     <t>CBM</t>
   </si>
   <si>
-    <t>68159910</t>
-  </si>
-  <si>
     <t>material</t>
   </si>
   <si>
-    <t>TAMARA</t>
+    <t>BLOCKS</t>
+  </si>
+  <si>
+    <t>SOFT BLOCKS</t>
   </si>
   <si>
     <t>IT</t>
@@ -181,9 +172,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="G3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +471,7 @@
     <col min="8" max="8" width="4.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -513,56 +502,50 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2">
+        <v>638271023</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
       </c>
       <c r="G2">
         <v>3650</v>
       </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>16200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on hrms permissions and servie orders
</commit_message>
<xml_diff>
--- a/dataTemplate/itemsExcelSample.xlsx
+++ b/dataTemplate/itemsExcelSample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Category</t>
   </si>
@@ -87,13 +87,19 @@
   </si>
   <si>
     <t>service</t>
+  </si>
+  <si>
+    <t>Work Type</t>
+  </si>
+  <si>
+    <t>Brickwork (Masonry)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +122,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,12 +175,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -453,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="A3:G3"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,9 +484,10 @@
     <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -502,8 +518,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -525,8 +544,11 @@
       <c r="G2">
         <v>3650</v>
       </c>
+      <c r="K2" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>